<commit_message>
Language and Country service changes a/c to  swagger 2.0.4
</commit_message>
<xml_diff>
--- a/TestResults/AffilTypePost.xlsx
+++ b/TestResults/AffilTypePost.xlsx
@@ -47,10 +47,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>TC_01</t>
-  </si>
-  <si>
-    <t>Verify that the GeoplAffilType service is successfully created when valid values are passed for all attributes in JSON Request.</t>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>Verify that the ERROR message is received when missing HTTP Header X-CSR-SECURITY_TOKEN.</t>
   </si>
   <si>
     <t>Post</t>
@@ -64,51 +64,51 @@
 	},
 	"geopoliticalAffiliationType":
 	{
-		"affilTypeCode":"AffilTest",
-		"affilTypeName":"AffilSpecCharTest"
+		"affiliationTypeCode":"aaa",
+		"affiliationTypeName":"Affilcodttt"
 	}
 }</t>
   </si>
   <si>
     <t xml:space="preserve">Input_UserName: 3791813
-Response_AffiliationTypeId: 5899303723994989864
-Input_affilTypeCode: AffilTest
-Input_affilTypeName: AffilSpecCharTest
-Input_LastUpdateUserName: 3791813
+Input_affiliationTypeCode: aaa
+Input_affiliationTypeName: Affilcodttt
 </t>
   </si>
   <si>
-    <t xml:space="preserve">DB_UserName: 3791813
-DB_AffiliationTypeId: 5899303723994989864
-DB_affilTypeCode: AffilTest
-DB_affilTypeName: AffilSpecCharTest
-DB_LastUpdateUserName: 3791813
-</t>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>401</t>
   </si>
   <si>
     <t xml:space="preserve">
 {
 	"meta":
 	{
-		"userName":"3791813",
 		"version":"1.0.0",
+		"timeStamp":"2020-06-22T09:32:53.175+0000",
+		"statusCode":"401",
 		"message":
 		{
-			"status":"SUCCESS",
-			"internalMessage":"GeoplAffilType Details successfully saved with affilTypeId :5899303723994989864",
-			"data":null
+			"status":"ERROR",
+			"internalMessage":"Security Error",
+			"data":
+			{
+				"errorMessage":"Exception occurred in Security Filter"
+			}
 		}
 	},
-	"data":
-	{
-		"affilTypeId":5899303723994989864
-	}
+	"errors":
+	[
+		{
+			"fieldName":"NA",
+			"message":"Missing HTTP header X-CSR-SECURITY_TOKEN"
+		}
+	]
 }</t>
   </si>
   <si>

</xml_diff>